<commit_message>
Made some changes for 7/26 deliverable
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_25_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 07_25_2019.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodney.feddema\Documents\GitHub\SD_County_LowFlow\0 - Field Data Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\work\SD_County_LowFlow\0 - Field Data Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990A6BF9-6079-4655-A7B7-A3CB84144FA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$U$350</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G49" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="G49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F237" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F237" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F248" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="F248" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F269" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="F269" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G326" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="G326" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K372" authorId="0" shapeId="0" xr:uid="{31A8CB08-FB2E-4485-BFFC-62382E984FFC}">
+    <comment ref="K372" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1632,7 +1631,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -1808,7 +1807,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2150,15 +2149,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:U406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H404" sqref="H404"/>
+      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H388" sqref="H388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15144,9 +15143,7 @@
       <c r="F387" s="26" t="s">
         <v>482</v>
       </c>
-      <c r="H387" s="26">
-        <v>-999999</v>
-      </c>
+      <c r="H387" s="26"/>
       <c r="J387" s="26">
         <v>60</v>
       </c>
@@ -15715,149 +15712,149 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U350" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U350"/>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G37" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G39" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G40" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G41" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G42" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G43" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G44" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G45" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G47" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G48" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G61" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G62" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G64" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G65" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G66" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="G67" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="G69" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="G70" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="G71" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="G72" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="G73" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="G74" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="G75" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="G76" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="G77" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="G78" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="G79" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="G80" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="G81" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="G83" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="G85" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="G86" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="G87" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="G88" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="G89" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="G94" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="G103" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="G104" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="G105" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="G108" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="G110" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="G112" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="G113" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="G124" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="G125" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="G135" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="G136" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="G137" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="G138" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="G140" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="G141" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="G142" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="G144" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="G145" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="G146" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="G147" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="G148" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="G149" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="G150" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="G151" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="G152" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="G153" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="G154" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="G155" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="G156" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="G157" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="G158" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="G159" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="G160" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="G161" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="G162" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="G163" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="G164" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="G173" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="G174" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="G175" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="G176" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="G183" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="G189" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="G190" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="G201" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="G204" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="G205" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="G207" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="G208" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="G211" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="G237" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="G241" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="G248" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="G250" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="G252" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="G253" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="G254" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="G260" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="G265" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="G273" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="G277" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="G279" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="G280" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="G296" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="G301" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="G314" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="G317" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="G328" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="G329" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="G338" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="G342" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="G343" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="G345" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="G348" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="G357" r:id="rId131" xr:uid="{09E168E1-7C43-4E13-95A6-E43F4467A67D}"/>
-    <hyperlink ref="G361" r:id="rId132" xr:uid="{6AB717EC-D96A-4E61-A164-33898160B7BA}"/>
-    <hyperlink ref="G363" r:id="rId133" xr:uid="{82E6ECB0-1880-4D77-99E0-A4B53D708A39}"/>
-    <hyperlink ref="G368" r:id="rId134" xr:uid="{B25B1056-0952-45B9-B2CE-95A8FC39C533}"/>
-    <hyperlink ref="G369" r:id="rId135" xr:uid="{5E67BBF9-F27B-484B-A500-D612D938296C}"/>
-    <hyperlink ref="G370" r:id="rId136" xr:uid="{415B6BA5-59CF-44F6-AA79-6B64CA7F8B27}"/>
-    <hyperlink ref="G372" r:id="rId137" xr:uid="{85044938-25E1-4CFD-BBFA-D8042FFF809E}"/>
-    <hyperlink ref="G382" r:id="rId138" xr:uid="{85CAF43A-1E2D-44DA-A91A-01838E85A879}"/>
-    <hyperlink ref="G388" r:id="rId139" xr:uid="{22798952-6A10-4BC8-ACCA-7007584D3826}"/>
-    <hyperlink ref="G389" r:id="rId140" xr:uid="{15929180-E5CE-485A-BE89-C88E751C6C51}"/>
-    <hyperlink ref="G395" r:id="rId141" xr:uid="{6824B6D5-FFCD-4691-9DD7-738EE8F575E1}"/>
+    <hyperlink ref="G5" r:id="rId1"/>
+    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3"/>
+    <hyperlink ref="G8" r:id="rId4"/>
+    <hyperlink ref="G9" r:id="rId5"/>
+    <hyperlink ref="G10" r:id="rId6"/>
+    <hyperlink ref="G11" r:id="rId7"/>
+    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="G13" r:id="rId9"/>
+    <hyperlink ref="G14" r:id="rId10"/>
+    <hyperlink ref="G15" r:id="rId11"/>
+    <hyperlink ref="G16" r:id="rId12"/>
+    <hyperlink ref="G17" r:id="rId13"/>
+    <hyperlink ref="G18" r:id="rId14"/>
+    <hyperlink ref="G19" r:id="rId15"/>
+    <hyperlink ref="G21" r:id="rId16"/>
+    <hyperlink ref="G22" r:id="rId17"/>
+    <hyperlink ref="G23" r:id="rId18"/>
+    <hyperlink ref="G33" r:id="rId19"/>
+    <hyperlink ref="G34" r:id="rId20"/>
+    <hyperlink ref="G37" r:id="rId21"/>
+    <hyperlink ref="G39" r:id="rId22"/>
+    <hyperlink ref="G40" r:id="rId23"/>
+    <hyperlink ref="G41" r:id="rId24"/>
+    <hyperlink ref="G42" r:id="rId25"/>
+    <hyperlink ref="G43" r:id="rId26"/>
+    <hyperlink ref="G44" r:id="rId27"/>
+    <hyperlink ref="G45" r:id="rId28"/>
+    <hyperlink ref="G47" r:id="rId29"/>
+    <hyperlink ref="G48" r:id="rId30"/>
+    <hyperlink ref="G61" r:id="rId31"/>
+    <hyperlink ref="G62" r:id="rId32"/>
+    <hyperlink ref="G64" r:id="rId33"/>
+    <hyperlink ref="G65" r:id="rId34"/>
+    <hyperlink ref="G66" r:id="rId35"/>
+    <hyperlink ref="G67" r:id="rId36"/>
+    <hyperlink ref="G69" r:id="rId37"/>
+    <hyperlink ref="G70" r:id="rId38"/>
+    <hyperlink ref="G71" r:id="rId39"/>
+    <hyperlink ref="G72" r:id="rId40"/>
+    <hyperlink ref="G73" r:id="rId41"/>
+    <hyperlink ref="G74" r:id="rId42"/>
+    <hyperlink ref="G75" r:id="rId43"/>
+    <hyperlink ref="G76" r:id="rId44"/>
+    <hyperlink ref="G77" r:id="rId45"/>
+    <hyperlink ref="G78" r:id="rId46"/>
+    <hyperlink ref="G79" r:id="rId47"/>
+    <hyperlink ref="G80" r:id="rId48"/>
+    <hyperlink ref="G81" r:id="rId49"/>
+    <hyperlink ref="G83" r:id="rId50"/>
+    <hyperlink ref="G85" r:id="rId51"/>
+    <hyperlink ref="G86" r:id="rId52"/>
+    <hyperlink ref="G87" r:id="rId53"/>
+    <hyperlink ref="G88" r:id="rId54"/>
+    <hyperlink ref="G89" r:id="rId55"/>
+    <hyperlink ref="G94" r:id="rId56"/>
+    <hyperlink ref="G103" r:id="rId57"/>
+    <hyperlink ref="G104" r:id="rId58"/>
+    <hyperlink ref="G105" r:id="rId59"/>
+    <hyperlink ref="G108" r:id="rId60"/>
+    <hyperlink ref="G110" r:id="rId61"/>
+    <hyperlink ref="G112" r:id="rId62"/>
+    <hyperlink ref="G113" r:id="rId63"/>
+    <hyperlink ref="G124" r:id="rId64"/>
+    <hyperlink ref="G125" r:id="rId65"/>
+    <hyperlink ref="G135" r:id="rId66"/>
+    <hyperlink ref="G136" r:id="rId67"/>
+    <hyperlink ref="G137" r:id="rId68"/>
+    <hyperlink ref="G138" r:id="rId69"/>
+    <hyperlink ref="G140" r:id="rId70"/>
+    <hyperlink ref="G141" r:id="rId71"/>
+    <hyperlink ref="G142" r:id="rId72"/>
+    <hyperlink ref="G144" r:id="rId73"/>
+    <hyperlink ref="G145" r:id="rId74"/>
+    <hyperlink ref="G146" r:id="rId75"/>
+    <hyperlink ref="G147" r:id="rId76"/>
+    <hyperlink ref="G148" r:id="rId77"/>
+    <hyperlink ref="G149" r:id="rId78"/>
+    <hyperlink ref="G150" r:id="rId79"/>
+    <hyperlink ref="G151" r:id="rId80"/>
+    <hyperlink ref="G152" r:id="rId81"/>
+    <hyperlink ref="G153" r:id="rId82"/>
+    <hyperlink ref="G154" r:id="rId83"/>
+    <hyperlink ref="G155" r:id="rId84"/>
+    <hyperlink ref="G156" r:id="rId85"/>
+    <hyperlink ref="G157" r:id="rId86"/>
+    <hyperlink ref="G158" r:id="rId87"/>
+    <hyperlink ref="G159" r:id="rId88"/>
+    <hyperlink ref="G160" r:id="rId89"/>
+    <hyperlink ref="G161" r:id="rId90"/>
+    <hyperlink ref="G162" r:id="rId91"/>
+    <hyperlink ref="G163" r:id="rId92"/>
+    <hyperlink ref="G164" r:id="rId93"/>
+    <hyperlink ref="G173" r:id="rId94"/>
+    <hyperlink ref="G174" r:id="rId95"/>
+    <hyperlink ref="G175" r:id="rId96"/>
+    <hyperlink ref="G176" r:id="rId97"/>
+    <hyperlink ref="G183" r:id="rId98"/>
+    <hyperlink ref="G189" r:id="rId99"/>
+    <hyperlink ref="G190" r:id="rId100"/>
+    <hyperlink ref="G201" r:id="rId101"/>
+    <hyperlink ref="G204" r:id="rId102"/>
+    <hyperlink ref="G205" r:id="rId103"/>
+    <hyperlink ref="G207" r:id="rId104"/>
+    <hyperlink ref="G208" r:id="rId105"/>
+    <hyperlink ref="G211" r:id="rId106"/>
+    <hyperlink ref="G237" r:id="rId107"/>
+    <hyperlink ref="G241" r:id="rId108"/>
+    <hyperlink ref="G248" r:id="rId109"/>
+    <hyperlink ref="G250" r:id="rId110"/>
+    <hyperlink ref="G252" r:id="rId111"/>
+    <hyperlink ref="G253" r:id="rId112"/>
+    <hyperlink ref="G254" r:id="rId113"/>
+    <hyperlink ref="G260" r:id="rId114"/>
+    <hyperlink ref="G265" r:id="rId115"/>
+    <hyperlink ref="G273" r:id="rId116"/>
+    <hyperlink ref="G277" r:id="rId117"/>
+    <hyperlink ref="G279" r:id="rId118"/>
+    <hyperlink ref="G280" r:id="rId119"/>
+    <hyperlink ref="G296" r:id="rId120"/>
+    <hyperlink ref="G301" r:id="rId121"/>
+    <hyperlink ref="G314" r:id="rId122"/>
+    <hyperlink ref="G317" r:id="rId123"/>
+    <hyperlink ref="G328" r:id="rId124"/>
+    <hyperlink ref="G329" r:id="rId125"/>
+    <hyperlink ref="G338" r:id="rId126"/>
+    <hyperlink ref="G342" r:id="rId127"/>
+    <hyperlink ref="G343" r:id="rId128"/>
+    <hyperlink ref="G345" r:id="rId129"/>
+    <hyperlink ref="G348" r:id="rId130"/>
+    <hyperlink ref="G357" r:id="rId131"/>
+    <hyperlink ref="G361" r:id="rId132"/>
+    <hyperlink ref="G363" r:id="rId133"/>
+    <hyperlink ref="G368" r:id="rId134"/>
+    <hyperlink ref="G369" r:id="rId135"/>
+    <hyperlink ref="G370" r:id="rId136"/>
+    <hyperlink ref="G372" r:id="rId137"/>
+    <hyperlink ref="G382" r:id="rId138"/>
+    <hyperlink ref="G388" r:id="rId139"/>
+    <hyperlink ref="G389" r:id="rId140"/>
+    <hyperlink ref="G395" r:id="rId141"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId142"/>
@@ -15866,7 +15863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -16137,7 +16134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>